<commit_message>
2017-01-31 update: energy.gov - chunk 7
</commit_message>
<xml_diff>
--- a/www.eia.gov/electricity/monthly/xls/table_1_01.xlsx
+++ b/www.eia.gov/electricity/monthly/xls/table_1_01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eiaSAScomp\erus_share\EPM\Output\Monthly_Output\EPM_2016_10\EPM_2016_10P_Run_at_2016_12_22_094008\Output\XLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eiaSAScomp\erus_share\EPM\Output\Monthly_Output\EPM_2016_11\EPM_2016_11P_Run_at_2017_01_19_170034\Output\XLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,9 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
-  <si>
-    <t>Table 1.1. Net Generation by Energy Source:  Total (All Sectors), 2006-October 2016</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="42">
+  <si>
+    <t>Table 1.1. Net Generation by Energy Source:  Total (All Sectors), 2006-November 2016</t>
   </si>
   <si>
     <t>(Thousand Megawatthours)</t>
@@ -154,7 +154,7 @@
     <t>Year to Date</t>
   </si>
   <si>
-    <t>Rolling 12 Months Ending in October</t>
+    <t>Rolling 12 Months Ending in November</t>
   </si>
   <si>
     <t>Coal includes anthracite, bituminous, subbituminous, lignite, and waste coal; synthetic coal and refined coal; and beginning in 2011, coal-derived synthesis gas. Prior to 2011 coal-derived synthesis gas was included in Other Gases.
@@ -1109,7 +1109,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -3519,322 +3519,372 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="10">
+        <v>87000</v>
+      </c>
+      <c r="C53" s="10">
+        <v>1058</v>
+      </c>
+      <c r="D53" s="10">
+        <v>781</v>
+      </c>
+      <c r="E53" s="10">
+        <v>94586</v>
+      </c>
+      <c r="F53" s="10">
+        <v>1001</v>
+      </c>
+      <c r="G53" s="10">
+        <v>65179</v>
+      </c>
+      <c r="H53" s="10">
+        <v>18815</v>
+      </c>
+      <c r="I53" s="10">
+        <v>2642</v>
+      </c>
+      <c r="J53" s="10">
+        <v>25874</v>
+      </c>
+      <c r="K53" s="10">
+        <v>-607</v>
+      </c>
+      <c r="L53" s="10">
+        <v>1093</v>
+      </c>
+      <c r="M53" s="10">
+        <v>297422</v>
+      </c>
+      <c r="N53" s="10">
+        <v>1307</v>
+      </c>
+      <c r="O53" s="10">
+        <v>3766</v>
+      </c>
+      <c r="P53" s="10">
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="8"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="8"/>
-      <c r="O53" s="8"/>
-      <c r="P53" s="8"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
-        <v>2014</v>
-      </c>
-      <c r="B54" s="10">
-        <v>1337963</v>
-      </c>
-      <c r="C54" s="10">
-        <v>16367</v>
-      </c>
-      <c r="D54" s="10">
-        <v>10032</v>
-      </c>
-      <c r="E54" s="10">
-        <v>951218</v>
-      </c>
-      <c r="F54" s="10">
-        <v>9795</v>
-      </c>
-      <c r="G54" s="10">
-        <v>658663</v>
-      </c>
-      <c r="H54" s="10">
-        <v>218413</v>
-      </c>
-      <c r="I54" s="10">
-        <v>15280</v>
-      </c>
-      <c r="J54" s="10">
-        <v>214504</v>
-      </c>
-      <c r="K54" s="10">
-        <v>-5163</v>
-      </c>
-      <c r="L54" s="10">
-        <v>11083</v>
-      </c>
-      <c r="M54" s="10">
-        <v>3438154</v>
-      </c>
-      <c r="N54" s="10">
-        <v>9675</v>
-      </c>
-      <c r="O54" s="10">
-        <v>22756</v>
-      </c>
-      <c r="P54" s="10">
-        <v>24954</v>
-      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="8"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B55" s="10">
-        <v>1175676</v>
+        <v>1457090</v>
       </c>
       <c r="C55" s="10">
-        <v>15429</v>
+        <v>17330</v>
       </c>
       <c r="D55" s="10">
-        <v>9413</v>
+        <v>10807</v>
       </c>
       <c r="E55" s="10">
-        <v>1121469</v>
+        <v>1035571</v>
       </c>
       <c r="F55" s="10">
-        <v>11105</v>
+        <v>10869</v>
       </c>
       <c r="G55" s="10">
-        <v>667280</v>
+        <v>723803</v>
       </c>
       <c r="H55" s="10">
-        <v>206577</v>
+        <v>237038</v>
       </c>
       <c r="I55" s="10">
-        <v>21593</v>
+        <v>16659</v>
       </c>
       <c r="J55" s="10">
-        <v>216901</v>
+        <v>239932</v>
       </c>
       <c r="K55" s="10">
-        <v>-4526</v>
+        <v>-5694</v>
       </c>
       <c r="L55" s="10">
-        <v>11603</v>
+        <v>12244</v>
       </c>
       <c r="M55" s="10">
-        <v>3452520</v>
+        <v>3755649</v>
       </c>
       <c r="N55" s="10">
-        <v>12243</v>
+        <v>10467</v>
       </c>
       <c r="O55" s="10">
-        <v>30940</v>
+        <v>24780</v>
       </c>
       <c r="P55" s="10">
-        <v>33837</v>
+        <v>27126</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
+        <v>2015</v>
+      </c>
+      <c r="B56" s="10">
+        <v>1262903</v>
+      </c>
+      <c r="C56" s="10">
+        <v>16424</v>
+      </c>
+      <c r="D56" s="10">
+        <v>10128</v>
+      </c>
+      <c r="E56" s="10">
+        <v>1223705</v>
+      </c>
+      <c r="F56" s="10">
+        <v>12007</v>
+      </c>
+      <c r="G56" s="10">
+        <v>727544</v>
+      </c>
+      <c r="H56" s="10">
+        <v>225915</v>
+      </c>
+      <c r="I56" s="10">
+        <v>23323</v>
+      </c>
+      <c r="J56" s="10">
+        <v>243236</v>
+      </c>
+      <c r="K56" s="10">
+        <v>-4811</v>
+      </c>
+      <c r="L56" s="10">
+        <v>12800</v>
+      </c>
+      <c r="M56" s="10">
+        <v>3753174</v>
+      </c>
+      <c r="N56" s="10">
+        <v>13225</v>
+      </c>
+      <c r="O56" s="10">
+        <v>33447</v>
+      </c>
+      <c r="P56" s="10">
+        <v>36548</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
         <v>2016</v>
       </c>
-      <c r="B56" s="10">
-        <v>1034120</v>
-      </c>
-      <c r="C56" s="10">
-        <v>10470</v>
-      </c>
-      <c r="D56" s="10">
-        <v>9585</v>
-      </c>
-      <c r="E56" s="10">
-        <v>1189871</v>
-      </c>
-      <c r="F56" s="10">
-        <v>10986</v>
-      </c>
-      <c r="G56" s="10">
-        <v>668454</v>
-      </c>
-      <c r="H56" s="10">
-        <v>224406</v>
-      </c>
-      <c r="I56" s="10">
-        <v>31190</v>
-      </c>
-      <c r="J56" s="10">
-        <v>250358</v>
-      </c>
-      <c r="K56" s="10">
-        <v>-5326</v>
-      </c>
-      <c r="L56" s="10">
-        <v>11458</v>
-      </c>
-      <c r="M56" s="10">
-        <v>3435570</v>
-      </c>
-      <c r="N56" s="10">
-        <v>16974</v>
-      </c>
-      <c r="O56" s="10">
-        <v>45055</v>
-      </c>
-      <c r="P56" s="10">
-        <v>48164</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+      <c r="B57" s="10">
+        <v>1121120</v>
+      </c>
+      <c r="C57" s="10">
+        <v>11528</v>
+      </c>
+      <c r="D57" s="10">
+        <v>10366</v>
+      </c>
+      <c r="E57" s="10">
+        <v>1284457</v>
+      </c>
+      <c r="F57" s="10">
+        <v>11987</v>
+      </c>
+      <c r="G57" s="10">
+        <v>733632</v>
+      </c>
+      <c r="H57" s="10">
+        <v>243220</v>
+      </c>
+      <c r="I57" s="10">
+        <v>33832</v>
+      </c>
+      <c r="J57" s="10">
+        <v>276232</v>
+      </c>
+      <c r="K57" s="10">
+        <v>-5933</v>
+      </c>
+      <c r="L57" s="10">
+        <v>12550</v>
+      </c>
+      <c r="M57" s="10">
+        <v>3732992</v>
+      </c>
+      <c r="N57" s="10">
+        <v>18281</v>
+      </c>
+      <c r="O57" s="10">
+        <v>48820</v>
+      </c>
+      <c r="P57" s="10">
+        <v>52113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="8"/>
-      <c r="O57" s="8"/>
-      <c r="P57" s="8"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
-        <v>2015</v>
-      </c>
-      <c r="B58" s="10">
-        <v>1419424</v>
-      </c>
-      <c r="C58" s="10">
-        <v>17339</v>
-      </c>
-      <c r="D58" s="10">
-        <v>11336</v>
-      </c>
-      <c r="E58" s="10">
-        <v>1296861</v>
-      </c>
-      <c r="F58" s="10">
-        <v>13332</v>
-      </c>
-      <c r="G58" s="10">
-        <v>805783</v>
-      </c>
-      <c r="H58" s="10">
-        <v>247530</v>
-      </c>
-      <c r="I58" s="10">
-        <v>24005</v>
-      </c>
-      <c r="J58" s="10">
-        <v>263918</v>
-      </c>
-      <c r="K58" s="10">
-        <v>-5536</v>
-      </c>
-      <c r="L58" s="10">
-        <v>13981</v>
-      </c>
-      <c r="M58" s="10">
-        <v>4107972</v>
-      </c>
-      <c r="N58" s="10">
-        <v>13801</v>
-      </c>
-      <c r="O58" s="10">
-        <v>34666</v>
-      </c>
-      <c r="P58" s="10">
-        <v>37806</v>
-      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
+        <v>2015</v>
+      </c>
+      <c r="B59" s="10">
+        <v>1387523</v>
+      </c>
+      <c r="C59" s="10">
+        <v>17371</v>
+      </c>
+      <c r="D59" s="10">
+        <v>11276</v>
+      </c>
+      <c r="E59" s="10">
+        <v>1314743</v>
+      </c>
+      <c r="F59" s="10">
+        <v>13160</v>
+      </c>
+      <c r="G59" s="10">
+        <v>800907</v>
+      </c>
+      <c r="H59" s="10">
+        <v>248243</v>
+      </c>
+      <c r="I59" s="10">
+        <v>24355</v>
+      </c>
+      <c r="J59" s="10">
+        <v>264826</v>
+      </c>
+      <c r="K59" s="10">
+        <v>-5291</v>
+      </c>
+      <c r="L59" s="10">
+        <v>14017</v>
+      </c>
+      <c r="M59" s="10">
+        <v>4091130</v>
+      </c>
+      <c r="N59" s="10">
+        <v>13991</v>
+      </c>
+      <c r="O59" s="10">
+        <v>35150</v>
+      </c>
+      <c r="P59" s="10">
+        <v>38346</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="9">
         <v>2016</v>
       </c>
-      <c r="B59" s="10">
-        <v>1210842</v>
-      </c>
-      <c r="C59" s="10">
-        <v>12412</v>
-      </c>
-      <c r="D59" s="10">
-        <v>11049</v>
-      </c>
-      <c r="E59" s="10">
-        <v>1401884</v>
-      </c>
-      <c r="F59" s="10">
-        <v>12998</v>
-      </c>
-      <c r="G59" s="10">
-        <v>798351</v>
-      </c>
-      <c r="H59" s="10">
-        <v>266909</v>
-      </c>
-      <c r="I59" s="10">
-        <v>34490</v>
-      </c>
-      <c r="J59" s="10">
-        <v>303725</v>
-      </c>
-      <c r="K59" s="10">
-        <v>-5892</v>
-      </c>
-      <c r="L59" s="10">
-        <v>13883</v>
-      </c>
-      <c r="M59" s="10">
-        <v>4060651</v>
-      </c>
-      <c r="N59" s="10">
-        <v>18870</v>
-      </c>
-      <c r="O59" s="10">
-        <v>49920</v>
-      </c>
-      <c r="P59" s="10">
-        <v>53359</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" ht="237.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="B60" s="10">
+        <v>1210615</v>
+      </c>
+      <c r="C60" s="10">
+        <v>12475</v>
+      </c>
+      <c r="D60" s="10">
+        <v>11115</v>
+      </c>
+      <c r="E60" s="10">
+        <v>1394234</v>
+      </c>
+      <c r="F60" s="10">
+        <v>13097</v>
+      </c>
+      <c r="G60" s="10">
+        <v>803266</v>
+      </c>
+      <c r="H60" s="10">
+        <v>266386</v>
+      </c>
+      <c r="I60" s="10">
+        <v>35402</v>
+      </c>
+      <c r="J60" s="10">
+        <v>303264</v>
+      </c>
+      <c r="K60" s="10">
+        <v>-6214</v>
+      </c>
+      <c r="L60" s="10">
+        <v>13779</v>
+      </c>
+      <c r="M60" s="10">
+        <v>4057419</v>
+      </c>
+      <c r="N60" s="10">
+        <v>19195</v>
+      </c>
+      <c r="O60" s="10">
+        <v>51179</v>
+      </c>
+      <c r="P60" s="10">
+        <v>54597</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="237.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="11"/>
-      <c r="M60" s="11"/>
-      <c r="N60" s="11"/>
-      <c r="O60" s="11"/>
-      <c r="P60" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="11"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="11"/>
+      <c r="O61" s="11"/>
+      <c r="P61" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A29:P29"/>
     <mergeCell ref="A42:P42"/>
-    <mergeCell ref="A53:P53"/>
-    <mergeCell ref="A57:P57"/>
-    <mergeCell ref="A60:P60"/>
+    <mergeCell ref="A54:P54"/>
+    <mergeCell ref="A58:P58"/>
+    <mergeCell ref="A61:P61"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
     <mergeCell ref="B3:M3"/>

</xml_diff>